<commit_message>
Use Case 4 complete - all 6 scenarios
</commit_message>
<xml_diff>
--- a/Use_cases.xlsx
+++ b/Use_cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\Desktop\Syracuse_MIS\IST 659\sql_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6164A29D-4AC8-406C-9ACC-67CDD8AC2EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520EC02B-797D-4178-BF1C-C2CD89FCFBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="4" xr2:uid="{861367E2-5E7E-4874-A518-0E67ACA05C83}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{861367E2-5E7E-4874-A518-0E67ACA05C83}"/>
   </bookViews>
   <sheets>
     <sheet name="Search Players" sheetId="2" r:id="rId1"/>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256F91A9-3538-4D71-B8AE-B13F230DBB06}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2271,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0642F3-05E9-4D16-8264-F0199B26322E}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
updated sql, use cases, and a new exel file with table column names
</commit_message>
<xml_diff>
--- a/Use_cases.xlsx
+++ b/Use_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\Desktop\Syracuse_MIS\IST 659\sql_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520EC02B-797D-4178-BF1C-C2CD89FCFBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE90B6C-A42D-4166-9099-B51FEEB7229D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{861367E2-5E7E-4874-A518-0E67ACA05C83}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
   <si>
     <t>Player Type</t>
   </si>
@@ -225,9 +225,6 @@
     <t>4. Will need to use a table variable</t>
   </si>
   <si>
-    <t>NOTE:  Cannot enter data into grayed out cells.  Number of entries opens/closes rows.  Must remove data from white rows before lowering number of entries</t>
-  </si>
-  <si>
     <t>Returns 1 or more graded cards based on selection criteria</t>
   </si>
   <si>
@@ -298,13 +295,25 @@
   </si>
   <si>
     <t>Reg% Jack%</t>
+  </si>
+  <si>
+    <t>NOTE:  Cannot enter data into grayed out cells.  Number of entries opens/closes rows.</t>
+  </si>
+  <si>
+    <t>TESTING BILLS UPSERT2</t>
+  </si>
+  <si>
+    <t>TESTING BILLS UPSERT</t>
+  </si>
+  <si>
+    <t>Player ID (if player card)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +377,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="4"/>
+      <color rgb="FF09885A"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -395,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -433,86 +448,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -540,21 +480,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,6 +589,251 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1158240</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>120161</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CB6A0AF-885B-49B0-AFEE-AE05C0EA486A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="2072640"/>
+          <a:ext cx="1104900" cy="424961"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1120140</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>21101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C02A1B0C-1521-44B1-A0EF-861EA88CF2C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6431280" y="1242060"/>
+          <a:ext cx="1104900" cy="424961"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>34290</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1139190</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D75C7C7-B0F4-47CE-AD25-7CB81033B533}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7280910" y="1287780"/>
+          <a:ext cx="1104900" cy="424961"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1127760</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>59201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE080DE0-28A0-4C5E-920B-D2C4AC9ED861}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5532120" y="3474720"/>
+          <a:ext cx="1104900" cy="424961"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7621</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>11431</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>74441</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B7109CB-7AB5-CECE-682A-AF8D53162903}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7940041" y="1485900"/>
+          <a:ext cx="1104900" cy="424961"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -953,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7206513D-6DD4-4E49-87B4-742BF236B492}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1011,259 +1191,260 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="2" t="s">
+    <row r="15" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B13" s="5" t="s">
+    <row r="16" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D16" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="F16" s="4">
         <v>1973</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C14"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16"/>
-      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C17"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="7" t="s">
+      <c r="C18"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D22" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E22" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F23" s="1">
         <v>1970</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
         <v>2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="1">
-        <f>F20+1</f>
+      <c r="F24" s="1">
+        <f>F23+1</f>
         <v>1971</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22"/>
-      <c r="F22" s="1">
-        <f t="shared" ref="F22:F39" si="0">F21+1</f>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C25"/>
+      <c r="F25" s="1">
+        <f t="shared" ref="F25:F42" si="0">F24+1</f>
         <v>1972</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23"/>
-      <c r="F23" s="1">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26"/>
+      <c r="F26" s="1">
         <f t="shared" si="0"/>
         <v>1973</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F25" s="1">
-        <f t="shared" si="0"/>
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F26" s="1">
-        <f t="shared" si="0"/>
-        <v>1976</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>1977</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>1978</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>1979</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>1980</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>1981</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>1982</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F33" s="1">
         <f t="shared" si="0"/>
-        <v>1983</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>1984</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F35" s="1">
         <f t="shared" si="0"/>
-        <v>1985</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="36" spans="6:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F36" s="1">
         <f t="shared" si="0"/>
-        <v>1986</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="37" spans="6:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F37" s="1">
         <f t="shared" si="0"/>
-        <v>1987</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="38" spans="6:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F38" s="1">
         <f t="shared" si="0"/>
-        <v>1988</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="39" spans="6:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F39" s="1">
         <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F40" s="1">
+        <f t="shared" si="0"/>
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41" s="1">
+        <f t="shared" si="0"/>
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42" s="1">
+        <f t="shared" si="0"/>
         <v>1989</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F13">
+  <conditionalFormatting sqref="F16">
     <cfRule type="expression" dxfId="11" priority="2">
-      <formula>$C$13&lt;&gt;"Stats"</formula>
+      <formula>$C$16&lt;&gt;"Stats"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F12">
+  <conditionalFormatting sqref="F15">
     <cfRule type="expression" dxfId="10" priority="1">
-      <formula>$C$13&lt;&gt;"Stats"</formula>
+      <formula>$C$16&lt;&gt;"Stats"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{C1184365-E4D1-4D93-B31B-52C47C347E15}">
-      <formula1>$B$19:$B$21</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{C1184365-E4D1-4D93-B31B-52C47C347E15}">
+      <formula1>$B$22:$B$24</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13" xr:uid="{D9E0CABD-CA12-4143-9E75-AD7CA5AF30D6}">
-      <formula1>$F$19:$F$39</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16" xr:uid="{D9E0CABD-CA12-4143-9E75-AD7CA5AF30D6}">
+      <formula1>$F$22:$F$42</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{97DA15B7-1A48-46E6-A948-E921DAE5FF54}">
-      <formula1>$C$19:$C$21</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{97DA15B7-1A48-46E6-A948-E921DAE5FF54}">
+      <formula1>$C$22:$C$24</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DC96B3-D483-4492-A9A7-2D65F1552FBC}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1316,55 +1497,49 @@
       <c r="D7"/>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B9" s="4">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="C9" s="4">
-        <v>100</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4">
-        <v>180</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1970</v>
-      </c>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8"/>
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="4">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C12" s="4">
+        <v>100</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
+        <v>180</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1970</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C13"/>
@@ -1373,179 +1548,173 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
-      <c r="F16" s="1">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17" s="1">
-        <f>F16+1</f>
-        <v>1971</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18" s="1">
-        <f t="shared" ref="F18:F35" si="0">F17+1</f>
-        <v>1972</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>1973</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <f>F19+1</f>
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="F21:F38" si="0">F20+1</f>
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>1976</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>1977</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>1978</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>1981</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>1982</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>1983</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>1984</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>1985</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>1986</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.55000000000000004">
@@ -1553,7 +1722,7 @@
       <c r="E33"/>
       <c r="F33" s="1">
         <f t="shared" si="0"/>
-        <v>1987</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.55000000000000004">
@@ -1561,7 +1730,7 @@
       <c r="E34"/>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
-        <v>1988</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.55000000000000004">
@@ -1569,26 +1738,51 @@
       <c r="E35"/>
       <c r="F35" s="1">
         <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36" s="1">
+        <f t="shared" si="0"/>
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37" s="1">
+        <f t="shared" si="0"/>
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38" s="1">
+        <f t="shared" si="0"/>
         <v>1989</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9" xr:uid="{4E2EF956-B54F-4DD5-8DAA-F92D4AE492E4}">
-      <formula1>$F$15:$F$35</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12" xr:uid="{4E2EF956-B54F-4DD5-8DAA-F92D4AE492E4}">
+      <formula1>$F$18:$F$38</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5595E9-97A3-4534-BD4B-E4C615A47201}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1634,58 +1828,52 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B9" s="4">
+    <row r="12" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B12" s="4">
         <v>0.28499999999999998</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C12" s="4">
         <v>15</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D12" s="4">
         <v>110</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
         <v>120</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G12" s="10">
         <v>1973</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="D13"/>
@@ -1693,207 +1881,223 @@
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="D16"/>
       <c r="E16"/>
-      <c r="G16" s="1">
-        <v>1970</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="G17" s="1">
-        <f>G16+1</f>
-        <v>1971</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="G18" s="1">
-        <f t="shared" ref="G18:G35" si="0">G17+1</f>
-        <v>1972</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="D19"/>
       <c r="E19"/>
       <c r="G19" s="1">
-        <f t="shared" si="0"/>
-        <v>1973</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20"/>
       <c r="E20"/>
       <c r="G20" s="1">
-        <f t="shared" si="0"/>
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <f>G19+1</f>
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21"/>
       <c r="E21"/>
       <c r="G21" s="1">
-        <f t="shared" si="0"/>
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="G21:G38" si="0">G20+1</f>
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22"/>
       <c r="E22"/>
       <c r="G22" s="1">
         <f t="shared" si="0"/>
-        <v>1976</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E23"/>
       <c r="G23" s="1">
         <f t="shared" si="0"/>
-        <v>1977</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E24"/>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>1978</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E25"/>
       <c r="G25" s="1">
         <f t="shared" si="0"/>
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E26"/>
       <c r="G26" s="1">
         <f t="shared" si="0"/>
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E27"/>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
-        <v>1981</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E28"/>
       <c r="G28" s="1">
         <f t="shared" si="0"/>
-        <v>1982</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E29"/>
       <c r="G29" s="1">
         <f t="shared" si="0"/>
-        <v>1983</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E30"/>
       <c r="G30" s="1">
         <f t="shared" si="0"/>
-        <v>1984</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E31"/>
       <c r="G31" s="1">
         <f t="shared" si="0"/>
-        <v>1985</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.55000000000000004">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E32"/>
       <c r="G32" s="1">
         <f t="shared" si="0"/>
-        <v>1986</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E33"/>
       <c r="G33" s="1">
         <f t="shared" si="0"/>
-        <v>1987</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E34"/>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
-        <v>1988</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E35"/>
       <c r="G35" s="1">
         <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E36"/>
+      <c r="G36" s="1">
+        <f t="shared" si="0"/>
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E37"/>
+      <c r="G37" s="1">
+        <f t="shared" si="0"/>
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E38"/>
+      <c r="G38" s="1">
+        <f t="shared" si="0"/>
         <v>1989</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9" xr:uid="{6F7C2E9B-7240-4AA7-AAC1-86F2E89DD543}">
-      <formula1>$G$15:$G$35</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G12" xr:uid="{6F7C2E9B-7240-4AA7-AAC1-86F2E89DD543}">
+      <formula1>$G$18:$G$38</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256F91A9-3538-4D71-B8AE-B13F230DBB06}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1909,7 +2113,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1919,41 +2123,41 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="16" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="21" t="s">
+      <c r="B11" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>75</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1961,13 +2165,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1975,13 +2179,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -1989,13 +2193,13 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2003,13 +2207,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2017,13 +2221,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2031,57 +2235,42 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B24" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B21" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="C24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B25"/>
@@ -2089,496 +2278,574 @@
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="7" t="s">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B29" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C32" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="1">
-        <v>1972</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="1">
-        <f>E28+1</f>
-        <v>1973</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30"/>
-      <c r="C30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="1">
-        <f t="shared" ref="E30:E31" si="0">E29+1</f>
-        <v>1974</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="E31" s="1">
-        <f t="shared" si="0"/>
-        <v>1975</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E32" s="1">
         <f>E31+1</f>
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33"/>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" ref="E33:E34" si="0">E32+1</f>
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="E34" s="1">
+        <f t="shared" si="0"/>
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E35" s="1">
+        <f>E34+1</f>
         <v>1976</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E33" s="1">
-        <f t="shared" ref="E33:E45" si="1">E32+1</f>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E36" s="1">
+        <f t="shared" ref="E36:E48" si="1">E35+1</f>
         <v>1977</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E34" s="1">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E37" s="1">
         <f t="shared" si="1"/>
         <v>1978</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E35" s="1">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E38" s="1">
         <f t="shared" si="1"/>
         <v>1979</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E36" s="1">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E39" s="1">
         <f t="shared" si="1"/>
         <v>1980</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E37" s="1">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E40" s="1">
         <f t="shared" si="1"/>
         <v>1981</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E38" s="1">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E41" s="1">
         <f t="shared" si="1"/>
         <v>1982</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E39" s="1">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E42" s="1">
         <f t="shared" si="1"/>
         <v>1983</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E40" s="1">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E43" s="1">
         <f t="shared" si="1"/>
         <v>1984</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E41" s="1">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E44" s="1">
         <f t="shared" si="1"/>
         <v>1985</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E42" s="1">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E45" s="1">
         <f t="shared" si="1"/>
         <v>1986</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E43" s="1">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E46" s="1">
         <f t="shared" si="1"/>
         <v>1987</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E44" s="1">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E47" s="1">
         <f t="shared" si="1"/>
         <v>1988</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E45" s="1">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E48" s="1">
         <f t="shared" si="1"/>
         <v>1989</v>
       </c>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E47" s="1"/>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E50" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{B75C9B01-306D-4D1C-8102-4C8A3DD7703D}">
-      <formula1>$B$27:$B$29</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24" xr:uid="{B75C9B01-306D-4D1C-8102-4C8A3DD7703D}">
+      <formula1>$B$30:$B$32</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21" xr:uid="{5E95D6F9-1E2E-405A-8C2F-948F363977D2}">
-      <formula1>$E$27:$E$46</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24" xr:uid="{5E95D6F9-1E2E-405A-8C2F-948F363977D2}">
+      <formula1>$E$30:$E$49</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21" xr:uid="{86EB2C91-59E9-4362-A49B-E7C680227343}">
-      <formula1>$C$27:$C$30</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{86EB2C91-59E9-4362-A49B-E7C680227343}">
+      <formula1>$C$30:$C$33</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0642F3-05E9-4D16-8264-F0199B26322E}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="6" width="18.26171875" customWidth="1"/>
+    <col min="1" max="1" width="16.734375" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="11.3125" customWidth="1"/>
+    <col min="4" max="4" width="11.26171875" customWidth="1"/>
+    <col min="5" max="5" width="22.83984375" customWidth="1"/>
+    <col min="6" max="6" width="18.26171875" customWidth="1"/>
     <col min="7" max="7" width="15.20703125" customWidth="1"/>
     <col min="8" max="10" width="18.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>60</v>
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="10" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="13" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="20" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" t="s">
+      <c r="B11" s="14">
+        <v>2</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.7" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>25</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>56</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>57</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>25</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="15" t="s">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="28.8" collapsed="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B14" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C14" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D14" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F14" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G14" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H14" s="19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="18"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="18"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="18"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="18"/>
+      <c r="I14" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="12">
+        <v>1234567890</v>
+      </c>
+      <c r="B15" s="12">
+        <v>1234567890</v>
+      </c>
+      <c r="C15" s="12">
+        <v>555</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1986</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="12">
+        <v>9</v>
+      </c>
+      <c r="G15" s="12">
+        <v>23</v>
+      </c>
+      <c r="H15" s="12">
+        <v>6</v>
+      </c>
+      <c r="I15" s="12">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="12">
+        <v>1111111</v>
+      </c>
+      <c r="B16" s="12">
+        <v>2222222</v>
+      </c>
+      <c r="C16" s="12">
+        <v>666</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1986</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="G16" s="12">
+        <v>45</v>
+      </c>
+      <c r="H16" s="12">
+        <v>10</v>
+      </c>
+      <c r="I16" s="12">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="12"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="18"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="18"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="18"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="19"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="18"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="19"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="18"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
-      <c r="H22" s="19"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="18"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
-      <c r="H23" s="19"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A14:H14">
+  <conditionalFormatting sqref="A15:I15">
     <cfRule type="expression" dxfId="9" priority="10">
-      <formula>$B$10&lt;1</formula>
+      <formula>$B$11&lt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:H16">
+  <conditionalFormatting sqref="A17:I17">
     <cfRule type="expression" dxfId="8" priority="9">
-      <formula>$B$10&lt;3</formula>
+      <formula>$B$11&lt;3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:H15">
+  <conditionalFormatting sqref="A16:I16">
     <cfRule type="expression" dxfId="7" priority="8">
-      <formula>$B$10&lt;2</formula>
+      <formula>$B$11&lt;2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:H17">
+  <conditionalFormatting sqref="A18:I18">
     <cfRule type="expression" dxfId="6" priority="7">
-      <formula>$B$10&lt;4</formula>
+      <formula>$B$11&lt;4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:H18">
+  <conditionalFormatting sqref="A19:I19">
     <cfRule type="expression" dxfId="5" priority="6">
-      <formula>$B$10&lt;5</formula>
+      <formula>$B$11&lt;5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:H19">
+  <conditionalFormatting sqref="A20:I20">
     <cfRule type="expression" dxfId="4" priority="5">
-      <formula>$B$10&lt;6</formula>
+      <formula>$B$11&lt;6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H20">
+  <conditionalFormatting sqref="A21:I21">
     <cfRule type="expression" dxfId="3" priority="4">
-      <formula>$B$10&lt;7</formula>
+      <formula>$B$11&lt;7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:H21">
+  <conditionalFormatting sqref="A22:I22">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$B$10&lt;8</formula>
+      <formula>$B$11&lt;8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22:H22">
+  <conditionalFormatting sqref="A23:I23">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$B$10&lt;9</formula>
+      <formula>$B$11&lt;9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:H23">
+  <conditionalFormatting sqref="A24:I24">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$B$10&lt;10</formula>
+      <formula>$B$11&lt;10</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{F6F4055F-B19A-4230-84A1-C7F27006CC5B}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{F6F4055F-B19A-4230-84A1-C7F27006CC5B}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A14:H14" xr:uid="{4651CBCA-FA3A-4AFB-B572-81EEB3098844}">
-      <formula1>$B$10&gt;=1</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A15:I15" xr:uid="{4651CBCA-FA3A-4AFB-B572-81EEB3098844}">
+      <formula1>$B$11&gt;=1</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A15:H15" xr:uid="{99702618-4F56-45C8-AB35-3448B09D8A3F}">
-      <formula1>$B$10&gt;=2</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A16:I16" xr:uid="{99702618-4F56-45C8-AB35-3448B09D8A3F}">
+      <formula1>$B$11&gt;=2</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A16:H16" xr:uid="{5B7A89B3-91D6-4488-8AE8-CED55FB3CBAC}">
-      <formula1>$B$10&gt;=3</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A17:I17" xr:uid="{5B7A89B3-91D6-4488-8AE8-CED55FB3CBAC}">
+      <formula1>$B$11&gt;=3</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A17:H17" xr:uid="{55EA1093-998C-4F2D-80DE-4AA6BA7F2351}">
-      <formula1>$B$10&gt;=4</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A18:I18" xr:uid="{55EA1093-998C-4F2D-80DE-4AA6BA7F2351}">
+      <formula1>$B$11&gt;=4</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A18:H18" xr:uid="{E9FA090A-1CA8-4A26-8066-2BB487C45E97}">
-      <formula1>$B$10&gt;=5</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A19:I19" xr:uid="{E9FA090A-1CA8-4A26-8066-2BB487C45E97}">
+      <formula1>$B$11&gt;=5</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A19:H19" xr:uid="{4041D56E-A858-4648-A9E2-77E411494908}">
-      <formula1>$B$10&gt;=6</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A20:I20" xr:uid="{4041D56E-A858-4648-A9E2-77E411494908}">
+      <formula1>$B$11&gt;=6</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A20:H20" xr:uid="{55495539-BCCF-467A-82E5-FADD9E333991}">
-      <formula1>$B$10&gt;=7</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A21:I21" xr:uid="{55495539-BCCF-467A-82E5-FADD9E333991}">
+      <formula1>$B$11&gt;=7</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A21:H21" xr:uid="{57E7712E-61E4-4B57-B4DF-7066052782C1}">
-      <formula1>$B$10&gt;=8</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A22:I22" xr:uid="{57E7712E-61E4-4B57-B4DF-7066052782C1}">
+      <formula1>$B$11&gt;=8</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A22:H22" xr:uid="{72221B6B-D946-4ADF-8406-1F6F3E3063F9}">
-      <formula1>$B$10&gt;=9</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A23:I23" xr:uid="{72221B6B-D946-4ADF-8406-1F6F3E3063F9}">
+      <formula1>$B$11&gt;=9</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A23:H23" xr:uid="{9256535F-BFF6-421A-AC97-BD9CC0E71A28}">
-      <formula1>$B$10&gt;=10</formula1>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Exceeds number of entries " error="Exceeds number of entries selected" sqref="A24:I24" xr:uid="{9256535F-BFF6-421A-AC97-BD9CC0E71A28}">
+      <formula1>$B$11&gt;=10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>